<commit_message>
Added tapered roller data and refactored tables
</commit_message>
<xml_diff>
--- a/Data/SKF_ballBearings.xlsx
+++ b/Data/SKF_ballBearings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uiano-my.sharepoint.com/personal/thomasls_uia_no/Documents/UiA/8. semester/MAS413/MAS413_Gearbox/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0FF9A74-2D98-4871-A60A-F60240D5978C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{C0FF9A74-2D98-4871-A60A-F60240D5978C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C4B41F0-D866-4081-B58F-81D8945D3F6C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EAFEB245-3773-4640-B7C2-CF509DF3A94D}"/>
   </bookViews>
@@ -909,12 +909,22 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.6" thickBot="1">
+    <row r="1" spans="1:8" ht="15.6" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -974,7 +984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29.4" thickBot="1">
+    <row r="4" spans="1:8" ht="15" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -998,7 +1008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29.4" thickBot="1">
+    <row r="5" spans="1:8" ht="15" thickBot="1">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1022,7 +1032,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="29.4" thickBot="1">
+    <row r="6" spans="1:8" ht="15" thickBot="1">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1046,7 +1056,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29.4" thickBot="1">
+    <row r="7" spans="1:8" ht="15" thickBot="1">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
@@ -1070,7 +1080,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.4" thickBot="1">
+    <row r="8" spans="1:8" ht="15" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
@@ -1094,7 +1104,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="29.4" thickBot="1">
+    <row r="9" spans="1:8" ht="15" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
@@ -1118,7 +1128,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29.4" thickBot="1">
+    <row r="10" spans="1:8" ht="15" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -1142,7 +1152,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="29.4" thickBot="1">
+    <row r="11" spans="1:8" ht="15" thickBot="1">
       <c r="A11" s="5" t="s">
         <v>52</v>
       </c>
@@ -1192,7 +1202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="29.4" thickBot="1">
+    <row r="13" spans="1:8" ht="15" thickBot="1">
       <c r="A13" s="5" t="s">
         <v>58</v>
       </c>
@@ -1216,7 +1226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="29.4" thickBot="1">
+    <row r="14" spans="1:8" ht="15" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>63</v>
       </c>
@@ -1240,7 +1250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="29.4" thickBot="1">
+    <row r="15" spans="1:8" ht="15" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>67</v>
       </c>
@@ -1264,7 +1274,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="29.4" thickBot="1">
+    <row r="16" spans="1:8" ht="15" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>70</v>
       </c>
@@ -1288,7 +1298,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29.4" thickBot="1">
+    <row r="17" spans="1:8" ht="15" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>75</v>
       </c>
@@ -1312,7 +1322,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="29.4" thickBot="1">
+    <row r="18" spans="1:8" ht="15" thickBot="1">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -1336,7 +1346,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="29.4" thickBot="1">
+    <row r="19" spans="1:8" ht="15" thickBot="1">
       <c r="A19" s="5" t="s">
         <v>85</v>
       </c>
@@ -1360,7 +1370,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="29.4" thickBot="1">
+    <row r="20" spans="1:8" ht="15" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>90</v>
       </c>
@@ -1384,7 +1394,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="29.4" thickBot="1">
+    <row r="21" spans="1:8" ht="15" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>94</v>
       </c>
@@ -1408,7 +1418,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="29.4" thickBot="1">
+    <row r="22" spans="1:8" ht="15" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>98</v>
       </c>
@@ -1432,7 +1442,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="29.4" thickBot="1">
+    <row r="23" spans="1:8" ht="15" thickBot="1">
       <c r="A23" s="8" t="s">
         <v>104</v>
       </c>

</xml_diff>